<commit_message>
seriously, the last one
</commit_message>
<xml_diff>
--- a/BOM/BOM_rev5_v3.xlsx
+++ b/BOM/BOM_rev5_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce57aa5d640eed3b/Documents/aa_School_Folders/Cat-Stuff/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="11_A5E4FF30ACB73D9F33323FDF55A22BDF50C3F669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55C7BBB3-D5E7-4E84-94AF-BA5DB13B8F6A}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="11_A5E4FF30ACB73D9F33323FDF55A22BDF50C3F669" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F599BF84-0FA6-44BD-AC43-682799A71516}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="177">
   <si>
     <t>Bill Of Material for:</t>
   </si>
@@ -485,9 +485,6 @@
     <t>P8.20KHCT-ND</t>
   </si>
   <si>
-    <t>Total for group</t>
-  </si>
-  <si>
     <t>Rev</t>
   </si>
   <si>
@@ -497,9 +494,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Total per member</t>
-  </si>
-  <si>
     <t>Initial BOM</t>
   </si>
   <si>
@@ -588,6 +582,9 @@
   </si>
   <si>
     <t>BOM revision # 3</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
   </si>
 </sst>
 </file>
@@ -632,7 +629,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -643,6 +640,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD0D0D0"/>
         <bgColor rgb="FFD0D0D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -745,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -784,17 +787,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,21 +1036,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.90625" customWidth="1"/>
-    <col min="2" max="2" width="40.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
-    <col min="4" max="4" width="23.6328125" customWidth="1"/>
-    <col min="5" max="5" width="30.90625" customWidth="1"/>
-    <col min="6" max="6" width="46.26953125" customWidth="1"/>
-    <col min="8" max="8" width="37.36328125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1"/>
@@ -1082,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1098,7 +1108,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1947,7 +1957,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1">
       <c r="A33" s="10">
         <v>1</v>
       </c>
@@ -1979,7 +1989,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1">
       <c r="A34" s="10">
         <v>1</v>
       </c>
@@ -2011,216 +2021,204 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A35" s="21">
+    <row r="35" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A35" s="20">
         <v>2</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="F35" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="I35" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="J35" s="24">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A36" s="22">
+        <v>1</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="E35" s="22" t="s">
+      <c r="D36" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="26">
+        <v>0.15</v>
+      </c>
+      <c r="J36" s="26">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A37" s="23">
+        <v>1</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="G37" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="F35" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="H35" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="I35" s="26">
+      <c r="H37" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="I37" s="26">
         <v>0.15</v>
       </c>
-      <c r="J35" s="26">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A36" s="23">
+      <c r="J37" s="26">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A38" s="23">
         <v>1</v>
       </c>
-      <c r="B36" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" s="24" t="s">
+      <c r="B38" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="G38" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H38" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="30">
-        <v>0.15</v>
-      </c>
-      <c r="J36" s="30">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A37" s="24">
+      <c r="I38" s="25">
+        <v>12.99</v>
+      </c>
+      <c r="J38" s="25">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A39" s="23">
         <v>1</v>
       </c>
-      <c r="B37" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="E37" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="F37" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="H37" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="I37" s="30">
-        <v>0.15</v>
-      </c>
-      <c r="J37" s="30">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A38" s="24">
-        <v>1</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="C38" s="24" t="s">
+      <c r="B39" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="E38" s="24" t="s">
+      <c r="D39" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="F38" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="G38" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="H38" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="I38" s="27">
-        <v>12.99</v>
-      </c>
-      <c r="J38" s="27">
-        <v>12.99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A39" s="24">
-        <v>1</v>
-      </c>
-      <c r="B39" s="25" t="s">
+      <c r="E39" s="23">
+        <v>4542</v>
+      </c>
+      <c r="F39" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="C39" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="25" t="s">
+      <c r="G39" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H39" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="24">
-        <v>4542</v>
-      </c>
-      <c r="F39" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="G39" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="H39" s="23" t="s">
+      <c r="I39" s="25">
+        <v>3.95</v>
+      </c>
+      <c r="J39" s="25">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1">
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="I39" s="27">
-        <v>3.95</v>
-      </c>
-      <c r="J39" s="27">
-        <v>3.95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="J40" s="13">
+      <c r="J40" s="32">
         <v>44.14</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="J41" s="13">
-        <v>11.04</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1">
+    <row r="41" spans="1:11" ht="15.75" customHeight="1">
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="30"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1">
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1">
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="30"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1">
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1">
+    <row r="45" spans="1:11" ht="15.75" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2232,7 +2230,7 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1">
+    <row r="46" spans="1:11" ht="15.75" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2244,7 +2242,7 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1">
+    <row r="47" spans="1:11" ht="15.75" customHeight="1">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2256,7 +2254,7 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1">
+    <row r="48" spans="1:11" ht="15.75" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2278,14 +2276,14 @@
     </row>
     <row r="50" spans="1:10" ht="15.75" customHeight="1">
       <c r="A50" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>145</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -2296,14 +2294,14 @@
     </row>
     <row r="51" spans="1:10" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B51" s="18">
         <v>45606</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -2312,27 +2310,27 @@
     </row>
     <row r="52" spans="1:10" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B52" s="18">
         <v>45609</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B53" s="19">
         <v>45615</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E53" s="3"/>
       <c r="I53" s="3"/>

</xml_diff>